<commit_message>
Se corrigió item en SelectCampania Modif de DataSourceMotor Se corrigió error con Item Refacturacion
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision AP No Enlatada.xlsx
+++ b/Sura/DataSource - Emision AP No Enlatada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CF4CC7-3177-4061-9725-6A7A8B7B7417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFDA8E0-958F-4F1A-80BE-DFA7F0836299}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="41">
   <si>
     <t>Usuario</t>
   </si>
@@ -146,13 +146,16 @@
   </si>
   <si>
     <t>https://preproducciongestion.segurossura.com.ar/pc/PolicyCenter.do</t>
+  </si>
+  <si>
+    <t>JUGADORES DE BASQUET</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,12 +177,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -263,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -272,69 +269,19 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -663,7 +610,7 @@
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +709,7 @@
       <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>9651159553</v>
       </c>
       <c r="F2">
@@ -793,7 +740,7 @@
         <v>16</v>
       </c>
       <c r="P2" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="Q2">
         <v>1</v>
@@ -805,32 +752,488 @@
         <v>21</v>
       </c>
       <c r="T2">
-        <v>21840809</v>
+        <v>21840810</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="5">
+        <v>9651159553</v>
+      </c>
+      <c r="F3">
+        <v>2302</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>550000</v>
+      </c>
+      <c r="S3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3">
+        <v>21840811</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="5">
+        <v>9651159553</v>
+      </c>
+      <c r="F4">
+        <v>2302</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>550000</v>
+      </c>
+      <c r="S4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T4">
+        <v>21840812</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="5">
+        <v>9651159553</v>
+      </c>
+      <c r="F5">
+        <v>2302</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>550000</v>
+      </c>
+      <c r="S5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T5">
+        <v>21840813</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="5">
+        <v>9651159553</v>
+      </c>
+      <c r="F6">
+        <v>2302</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" t="s">
+        <v>16</v>
+      </c>
+      <c r="P6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>550000</v>
+      </c>
+      <c r="S6" t="s">
+        <v>21</v>
+      </c>
+      <c r="T6">
+        <v>21840814</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="E7" s="4"/>
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="5">
+        <v>9651159553</v>
+      </c>
+      <c r="F7">
+        <v>2302</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" t="s">
+        <v>16</v>
+      </c>
+      <c r="P7" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>550000</v>
+      </c>
+      <c r="S7" t="s">
+        <v>21</v>
+      </c>
+      <c r="T7">
+        <v>21840815</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="E8" s="4"/>
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="5">
+        <v>9651159553</v>
+      </c>
+      <c r="F8">
+        <v>2302</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" t="s">
+        <v>16</v>
+      </c>
+      <c r="P8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>550000</v>
+      </c>
+      <c r="S8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T8">
+        <v>21840816</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="E9" s="4"/>
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="5">
+        <v>9651159553</v>
+      </c>
+      <c r="F9">
+        <v>2302</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" t="s">
+        <v>16</v>
+      </c>
+      <c r="P9" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>550000</v>
+      </c>
+      <c r="S9" t="s">
+        <v>21</v>
+      </c>
+      <c r="T9">
+        <v>21840817</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="E10" s="5"/>
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="5">
+        <v>9651159553</v>
+      </c>
+      <c r="F10">
+        <v>2302</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" t="s">
+        <v>16</v>
+      </c>
+      <c r="P10" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>550000</v>
+      </c>
+      <c r="S10" t="s">
+        <v>21</v>
+      </c>
+      <c r="T10">
+        <v>21840818</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
-      <c r="E11" s="5"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
-      <c r="E12" s="5"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
@@ -847,6 +1250,14 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{8E917A1D-8E8F-4045-A5F6-0187DE514284}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{9C71C1FF-D005-4D58-B92F-22957BB55CAE}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{32F2CFD8-4C06-4817-9C71-312F33357643}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{BEDB163D-EC02-44F6-82D1-82D89512A434}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{F4986BC8-F90C-4EFC-B8DD-B0215D6B8A63}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{AF0E9C2B-8066-4D5A-9D17-AB1401973A83}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{826BCC7A-0228-446A-AB9C-91D7D096B650}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{C80BBE0C-98F7-4244-8B51-367C26E6DCA1}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{6B3C252D-E6CB-4A07-9417-4EC1127F7881}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -875,7 +1286,7 @@
       <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="7">
+      <c r="E1" s="6">
         <v>6328381177</v>
       </c>
       <c r="H1" t="s">
@@ -915,56 +1326,56 @@
         <v>21840807</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:20" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>5944603681</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="8" t="s">
+      <c r="J2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" s="8" t="s">
+      <c r="O2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="8">
+      <c r="Q2" s="7">
         <v>1</v>
       </c>
-      <c r="R2" s="8">
+      <c r="R2" s="7">
         <v>400000</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="8">
+      <c r="T2" s="7">
         <v>21840805</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se modificaron Datos y de PC_gestionDocumental se creo el test run para emitir Motor Compl Blank Prendario y VariosAutos
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision AP No Enlatada.xlsx
+++ b/Sura/DataSource - Emision AP No Enlatada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A098B5D-6547-40B3-B066-D9D6B88E9A9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCECFBD-83B1-4931-8A1E-C08494D3B069}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +752,7 @@
         <v>21</v>
       </c>
       <c r="T2">
-        <v>21840819</v>
+        <v>21840820</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se agregó al TC: Emision_Motor 2 recording para que seleccione el grupo del PAS
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision AP No Enlatada.xlsx
+++ b/Sura/DataSource - Emision AP No Enlatada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0170B32D-3288-4A92-972A-157CF79AFEB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A7FAA9-1761-4B36-A1FA-35F9CDF17CBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="42">
   <si>
     <t>Usuario</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>JUGADORES DE BASQUET</t>
+  </si>
+  <si>
+    <t>CADETE EN MOTO</t>
   </si>
 </sst>
 </file>
@@ -609,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,7 +760,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>39</v>
@@ -769,7 +772,7 @@
         <v>26</v>
       </c>
       <c r="E3" s="5">
-        <v>9651159553</v>
+        <v>7105947778</v>
       </c>
       <c r="F3">
         <v>2302</v>
@@ -781,7 +784,7 @@
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
         <v>16</v>
@@ -799,7 +802,7 @@
         <v>16</v>
       </c>
       <c r="P3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q3">
         <v>1</v>
@@ -811,7 +814,7 @@
         <v>21</v>
       </c>
       <c r="T3">
-        <v>21840811</v>
+        <v>21004018</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se arregló rutas a C:temp se modificó el valor por defecto de la Franquicia Fija
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision AP No Enlatada.xlsx
+++ b/Sura/DataSource - Emision AP No Enlatada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07175DF-A935-486E-958A-AF3C5E7366AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3029E55C-0BDA-4423-AAE8-B487CFD14EF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -613,7 +613,7 @@
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +713,7 @@
         <v>26</v>
       </c>
       <c r="E2" s="5">
-        <v>7635954411</v>
+        <v>7105947778</v>
       </c>
       <c r="F2">
         <v>2302</v>
@@ -755,7 +755,7 @@
         <v>21</v>
       </c>
       <c r="T2">
-        <v>21004019</v>
+        <v>31200144</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>